<commit_message>
Rodei o Cosine e acrescentei um comment
</commit_message>
<xml_diff>
--- a/similaridade.xlsx
+++ b/similaridade.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PESSOAL\Desktop\TCC-main\TCC-main\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -261,8 +256,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,21 +320,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -377,9 +364,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,10 +398,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,10 +432,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -622,21 +607,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -655,10 +633,10 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>0.45536964310781641</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4553696431078164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -666,10 +644,10 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <v>0.58651184892078334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5865118489207833</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -680,7 +658,7 @@
         <v>0.4306635094099272</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -688,10 +666,10 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>0.44788737871373913</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4478873787137391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -699,10 +677,10 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>0.42536143078651872</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4253614307865187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -710,10 +688,10 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>0.42157533696557359</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4215753369655736</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -721,10 +699,10 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>0.41779597138595281</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4177959713859528</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -732,10 +710,10 @@
         <v>30</v>
       </c>
       <c r="C9">
-        <v>0.42423249393170248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4242324939317025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -743,10 +721,10 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>0.40703543037555268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4070354303755527</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -754,10 +732,10 @@
         <v>32</v>
       </c>
       <c r="C11">
-        <v>0.41045518743069859</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4104551874306986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -765,10 +743,10 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>0.41360326249328577</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4136032624932858</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -776,10 +754,10 @@
         <v>34</v>
       </c>
       <c r="C13">
-        <v>0.42652192415992579</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4265219241599258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -787,10 +765,10 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>0.40838875888894538</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4083887588889454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -798,10 +776,10 @@
         <v>36</v>
       </c>
       <c r="C15">
-        <v>0.46239803207832458</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4623980320783246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -809,10 +787,10 @@
         <v>37</v>
       </c>
       <c r="C16">
-        <v>0.40195142143356127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4019514214335613</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -823,7 +801,7 @@
         <v>0.4287942444104117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -831,10 +809,10 @@
         <v>39</v>
       </c>
       <c r="C18">
-        <v>0.51881007941737978</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5188100794173798</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -842,10 +820,10 @@
         <v>40</v>
       </c>
       <c r="C19">
-        <v>0.41846465377480291</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4184646537748029</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -853,10 +831,10 @@
         <v>41</v>
       </c>
       <c r="C20">
-        <v>0.46516335620248589</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4651633562024859</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -864,10 +842,10 @@
         <v>42</v>
       </c>
       <c r="C21">
-        <v>0.43444744299029109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4344474429902911</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -875,10 +853,10 @@
         <v>43</v>
       </c>
       <c r="C22">
-        <v>0.44878323306005619</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4487832330600562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -886,10 +864,10 @@
         <v>44</v>
       </c>
       <c r="C23">
-        <v>0.47563642485178542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4756364248517854</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -900,7 +878,7 @@
         <v>0.4476572665230627</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -911,7 +889,7 @@
         <v>0.4630488464916091</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -919,10 +897,10 @@
         <v>47</v>
       </c>
       <c r="C26">
-        <v>0.52107619219154511</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5210761921915451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -930,10 +908,10 @@
         <v>48</v>
       </c>
       <c r="C27">
-        <v>0.42104861986962189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4210486198696219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -941,10 +919,10 @@
         <v>49</v>
       </c>
       <c r="C28">
-        <v>0.48789016593104978</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4878901659310498</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -952,10 +930,10 @@
         <v>50</v>
       </c>
       <c r="C29">
-        <v>0.40095043561294352</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4009504356129435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -963,10 +941,10 @@
         <v>51</v>
       </c>
       <c r="C30">
-        <v>0.55513620996070034</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5551362099607003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -974,10 +952,10 @@
         <v>52</v>
       </c>
       <c r="C31">
-        <v>0.40237974348787903</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.402379743487879</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -985,10 +963,10 @@
         <v>53</v>
       </c>
       <c r="C32">
-        <v>0.42198439304175628</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4219843930417563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -996,10 +974,10 @@
         <v>54</v>
       </c>
       <c r="C33">
-        <v>0.43989406424209648</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4398940642420965</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1007,10 +985,10 @@
         <v>55</v>
       </c>
       <c r="C34">
-        <v>0.42657599358684201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.426575993586842</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1018,10 +996,10 @@
         <v>56</v>
       </c>
       <c r="C35">
-        <v>0.40422105057337188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4042210505733719</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1029,10 +1007,10 @@
         <v>57</v>
       </c>
       <c r="C36">
-        <v>0.49837886206514043</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4983788620651404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1040,10 +1018,10 @@
         <v>58</v>
       </c>
       <c r="C37">
-        <v>0.42609440555701877</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4260944055570188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1051,10 +1029,10 @@
         <v>59</v>
       </c>
       <c r="C38">
-        <v>0.41724506643381809</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4172450664338181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1062,10 +1040,10 @@
         <v>60</v>
       </c>
       <c r="C39">
-        <v>0.51922762744776474</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5192276274477647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1073,10 +1051,10 @@
         <v>61</v>
       </c>
       <c r="C40">
-        <v>0.50181824670952691</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5018182467095269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1084,10 +1062,10 @@
         <v>62</v>
       </c>
       <c r="C41">
-        <v>0.46392962576596808</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4639296257659681</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1076,7 @@
         <v>0.4195911377371116</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1106,10 +1084,10 @@
         <v>64</v>
       </c>
       <c r="C43">
-        <v>0.50447498628473841</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5044749862847384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -1117,10 +1095,10 @@
         <v>65</v>
       </c>
       <c r="C44">
-        <v>0.41163592901519003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.41163592901519</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1128,10 +1106,10 @@
         <v>66</v>
       </c>
       <c r="C45">
-        <v>0.45103861317359578</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4510386131735958</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1139,10 +1117,10 @@
         <v>67</v>
       </c>
       <c r="C46">
-        <v>0.46522471840392082</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4652247184039208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1150,10 +1128,10 @@
         <v>68</v>
       </c>
       <c r="C47">
-        <v>0.43981941298878469</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4398194129887847</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -1161,10 +1139,10 @@
         <v>69</v>
       </c>
       <c r="C48">
-        <v>0.47724809671667251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4772480967166725</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -1172,10 +1150,10 @@
         <v>70</v>
       </c>
       <c r="C49">
-        <v>0.43810436540243969</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4381043654024397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -1183,10 +1161,10 @@
         <v>71</v>
       </c>
       <c r="C50">
-        <v>0.52422259080724132</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5242225908072413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -1194,10 +1172,10 @@
         <v>72</v>
       </c>
       <c r="C51">
-        <v>0.54342846713969017</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5434284671396902</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -1208,7 +1186,7 @@
         <v>0.4330706194722248</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>21</v>
       </c>
@@ -1216,10 +1194,10 @@
         <v>74</v>
       </c>
       <c r="C53">
-        <v>0.55427015475749475</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5542701547574947</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -1227,10 +1205,10 @@
         <v>75</v>
       </c>
       <c r="C54">
-        <v>0.54895429388989836</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5489542938898984</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -1238,10 +1216,10 @@
         <v>76</v>
       </c>
       <c r="C55">
-        <v>0.46965594055800569</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4696559405580057</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1249,10 +1227,10 @@
         <v>77</v>
       </c>
       <c r="C56">
-        <v>0.49384297753824052</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.4938429775382405</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1260,7 +1238,7 @@
         <v>78</v>
       </c>
       <c r="C57">
-        <v>0.55848513925730181</v>
+        <v>0.5584851392573018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>